<commit_message>
API: Imports support question_id
</commit_message>
<xml_diff>
--- a/api/tests/imports/challenge/challenge_import_update_with_correct_answers.xlsx
+++ b/api/tests/imports/challenge/challenge_import_update_with_correct_answers.xlsx
@@ -16,66 +16,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="56">
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Short Description</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>Max Points</t>
-  </si>
-  <si>
-    <t>Starts At</t>
-  </si>
-  <si>
-    <t>Expires At</t>
-  </si>
-  <si>
-    <t>Hint Text</t>
-  </si>
-  <si>
-    <t>Hint Image</t>
-  </si>
-  <si>
-    <t>Skill Analytical</t>
-  </si>
-  <si>
-    <t>Skill StrategicPlanning</t>
-  </si>
-  <si>
-    <t>Skill Adaptability</t>
-  </si>
-  <si>
-    <t>Skill PremierLeagueKnowledge</t>
-  </si>
-  <si>
-    <t>Skill RiskManagement</t>
-  </si>
-  <si>
-    <t>Skill DecisionMakingUnderPressure</t>
-  </si>
-  <si>
-    <t>Skill FinancialManagement</t>
-  </si>
-  <si>
-    <t>Skill LongTermVision</t>
-  </si>
-  <si>
-    <t>Show Statistics Continuously</t>
-  </si>
-  <si>
-    <t>Gameweek</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="48">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>short_description</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>max_points</t>
+  </si>
+  <si>
+    <t>starts_at</t>
+  </si>
+  <si>
+    <t>expires_at</t>
+  </si>
+  <si>
+    <t>hint_text</t>
+  </si>
+  <si>
+    <t>hint_image</t>
+  </si>
+  <si>
+    <t>show_statistics_continuously</t>
+  </si>
+  <si>
+    <t>gameweek</t>
+  </si>
+  <si>
+    <t>skill_analytical</t>
+  </si>
+  <si>
+    <t>skill_strategicplanning</t>
+  </si>
+  <si>
+    <t>skill_adaptability</t>
+  </si>
+  <si>
+    <t>skill_premierleagueknowledge</t>
+  </si>
+  <si>
+    <t>skill_riskmanagement</t>
+  </si>
+  <si>
+    <t>skill_decisionmakingunderpressure</t>
+  </si>
+  <si>
+    <t>skill_financialmanagement</t>
+  </si>
+  <si>
+    <t>skill_longtermvision</t>
   </si>
   <si>
     <t>01933333-0000-7000-8000-000000000001</t>
@@ -105,46 +105,49 @@
     <t>https://example.com/hint.jpg</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Challenge ID</t>
-  </si>
-  <si>
-    <t>Text</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Numeric Type Min</t>
-  </si>
-  <si>
-    <t>Numeric Type Max</t>
-  </si>
-  <si>
-    <t>Choices</t>
-  </si>
-  <si>
-    <t>Choices Min Selections</t>
-  </si>
-  <si>
-    <t>Choices Max Selections</t>
-  </si>
-  <si>
-    <t>Correct Text Answer</t>
-  </si>
-  <si>
-    <t>Correct Numeric Answer</t>
-  </si>
-  <si>
-    <t>Correct Selected Choice Text</t>
-  </si>
-  <si>
-    <t>Correct Selected Choice Texts</t>
-  </si>
-  <si>
-    <t>Correct Ordered Choice Texts</t>
+    <t>question_id</t>
+  </si>
+  <si>
+    <t>challenge_id</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>numeric_type_min</t>
+  </si>
+  <si>
+    <t>numeric_type_max</t>
+  </si>
+  <si>
+    <t>choices</t>
+  </si>
+  <si>
+    <t>choices_min_selections</t>
+  </si>
+  <si>
+    <t>choices_max_selections</t>
+  </si>
+  <si>
+    <t>correct_text_answer</t>
+  </si>
+  <si>
+    <t>correct_numeric_answer</t>
+  </si>
+  <si>
+    <t>correct_selected_choice_text</t>
+  </si>
+  <si>
+    <t>correct_selected_choice_texts</t>
+  </si>
+  <si>
+    <t>correct_ordered_choice_texts</t>
+  </si>
+  <si>
+    <t>01933333-0000-7000-8000-000000000006</t>
   </si>
   <si>
     <t>Who will you transfer in as your premium midfielder?</t>
@@ -153,37 +156,10 @@
     <t>single_select</t>
   </si>
   <si>
-    <t>[{"text":"Mohamed Salah","description":"Liverpool star with great form","image":"https:\/\/example.com\/salah.jpg"},{"text":"Kevin De Bruyne","description":"Man City playmaker","image":null},{"text":"Bruno Fernandes","description":"Manchester United captain"}]</t>
+    <t>[{"text":"Mohamed Salah","description":"Liverpool star with great form","image":"https://example.com/salah.jpg"},{"text":"Kevin De Bruyne","description":"Man City playmaker"},{"text":"Bruno Fernandes","description":"Manchester United captain"}]</t>
   </si>
   <si>
     <t>Mohamed Salah</t>
-  </si>
-  <si>
-    <t>Select your defensive picks (choose 2)</t>
-  </si>
-  <si>
-    <t>multi_select</t>
-  </si>
-  <si>
-    <t>[{"text":"William Saliba","description":"Arsenal defender"},{"text":"Virgil van Dijk","description":"Liverpool defender"},{"text":"Ruben Dias","description":"Man City defender"},{"text":"Cristian Romero","description":"Spurs defender"}]</t>
-  </si>
-  <si>
-    <t>How many goals will your team score this gameweek?</t>
-  </si>
-  <si>
-    <t>numeric</t>
-  </si>
-  <si>
-    <t>Explain your transfer strategy in one sentence</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>https://example.com/strategy.jpg</t>
-  </si>
-  <si>
-    <t>Focus on form and fixtures</t>
   </si>
 </sst>
 </file>
@@ -625,34 +601,34 @@
         <v>28</v>
       </c>
       <c r="K2">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>15</v>
+        <v>0.25</v>
       </c>
       <c r="N2">
-        <v>40</v>
+        <v>0.3</v>
       </c>
       <c r="O2">
-        <v>20</v>
+        <v>0.15</v>
       </c>
       <c r="P2">
-        <v>25</v>
+        <v>0.4</v>
       </c>
       <c r="Q2">
-        <v>35</v>
+        <v>0.2</v>
       </c>
       <c r="R2">
-        <v>10</v>
-      </c>
-      <c r="S2" t="s">
-        <v>29</v>
+        <v>0.25</v>
+      </c>
+      <c r="S2">
+        <v>0.35</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -667,7 +643,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,128 +651,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>32</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
       </c>
-      <c r="H2">
-        <v>1</v>
+      <c r="H2" t="s">
+        <v>46</v>
       </c>
       <c r="I2">
         <v>1</v>
       </c>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="M2" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>50</v>
-      </c>
-      <c r="K4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>